<commit_message>
generated the data as clsx files instead of csv
</commit_message>
<xml_diff>
--- a/data/guatemala/analysis/flood_trigger_analysis_2025_10_3yr_lead3d.xlsx
+++ b/data/guatemala/analysis/flood_trigger_analysis_2025_10_3yr_lead3d.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X29"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2963,6 +2963,92 @@
         <v>-58.57919091170383</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Guatemala</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>guatemala</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Primary Station</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2025-10-29</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>3</v>
+      </c>
+      <c r="G30" t="n">
+        <v>14.22499999999995</v>
+      </c>
+      <c r="H30" t="n">
+        <v>-90.32499999999959</v>
+      </c>
+      <c r="I30" t="n">
+        <v>3</v>
+      </c>
+      <c r="J30" t="n">
+        <v>202.9380777444821</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
+      <c r="L30" t="n">
+        <v>171.182462054225</v>
+      </c>
+      <c r="M30" t="n">
+        <v>242.9454220724218</v>
+      </c>
+      <c r="N30" t="n">
+        <v>50</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>80.484375</v>
+      </c>
+      <c r="R30" t="n">
+        <v>80.58984375</v>
+      </c>
+      <c r="S30" t="n">
+        <v>79.4921875</v>
+      </c>
+      <c r="T30" t="n">
+        <v>83.46875</v>
+      </c>
+      <c r="U30" t="n">
+        <v>80.14453125</v>
+      </c>
+      <c r="V30" t="n">
+        <v>80.802734375</v>
+      </c>
+      <c r="W30" t="b">
+        <v>0</v>
+      </c>
+      <c r="X30" t="n">
+        <v>-60.34042704329874</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>